<commit_message>
unit test for import bios
</commit_message>
<xml_diff>
--- a/luffy/bios.xlsx
+++ b/luffy/bios.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
   <si>
     <t>BIOS ID</t>
   </si>
@@ -26,7 +26,10 @@
     <t>Test Type</t>
   </si>
   <si>
-    <t>Schedule</t>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>End</t>
   </si>
   <si>
     <t>BIOS Version</t>
@@ -50,7 +53,7 @@
     <t>BC Test</t>
   </si>
   <si>
-    <t>2019/06/18 - 2019/06/18</t>
+    <t>2019-06-18</t>
   </si>
   <si>
     <t>B.24</t>
@@ -92,7 +95,10 @@
     <t>BIOS pre-test</t>
   </si>
   <si>
-    <t>2019/06/08 - 2019/06/11</t>
+    <t>2019-06-08</t>
+  </si>
+  <si>
+    <t>2019-06-11</t>
   </si>
   <si>
     <t>F.10</t>
@@ -222,7 +228,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true" showGridLines="false" zoomScale="75">
       <pane ySplit="1.0" state="frozen" topLeftCell="A2" activePane="bottomLeft"/>
@@ -235,11 +241,12 @@
     <col min="2" max="2" width="20.0" customWidth="true"/>
     <col min="3" max="3" width="20.0" customWidth="true"/>
     <col min="4" max="4" width="30.0" customWidth="true"/>
-    <col min="5" max="5" width="40.0" customWidth="true"/>
-    <col min="6" max="6" width="20.0" customWidth="true"/>
-    <col min="7" max="7" width="30.0" customWidth="true"/>
-    <col min="8" max="8" width="40.0" customWidth="true"/>
-    <col min="9" max="9" width="20.0" customWidth="true"/>
+    <col min="5" max="5" width="30.0" customWidth="true"/>
+    <col min="6" max="6" width="30.0" customWidth="true"/>
+    <col min="7" max="7" width="20.0" customWidth="true"/>
+    <col min="8" max="8" width="30.0" customWidth="true"/>
+    <col min="9" max="9" width="40.0" customWidth="true"/>
+    <col min="10" max="10" width="20.0" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="true">
@@ -270,22 +277,25 @@
       <c r="I1" t="s" s="1">
         <v>8</v>
       </c>
+      <c r="J1" t="s" s="1">
+        <v>9</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
         <v>32.0</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F2" t="s">
         <v>13</v>
@@ -298,6 +308,9 @@
       </c>
       <c r="I2" t="s">
         <v>16</v>
+      </c>
+      <c r="J2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="3">
@@ -305,19 +318,19 @@
         <v>31.0</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F3" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="G3" t="s">
         <v>20</v>
@@ -327,6 +340,9 @@
       </c>
       <c r="I3" t="s">
         <v>22</v>
+      </c>
+      <c r="J3" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="4">
@@ -334,28 +350,31 @@
         <v>1.0</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I4" t="s">
-        <v>30</v>
+        <v>31</v>
+      </c>
+      <c r="J4" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>